<commit_message>
[WIP] Final experiments and results.
</commit_message>
<xml_diff>
--- a/paper/paper_cntf_coherence_results.xlsx
+++ b/paper/paper_cntf_coherence_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiagofilipesousagoncalves/Desktop/GitHub/proto-counterfactuals/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74593F77-225E-A447-BE97-CE9E75A18B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6131A1-E854-A741-A3EA-B110DED071BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CUB2002011" sheetId="1" r:id="rId1"/>
@@ -174,9 +174,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000_ "/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -241,53 +241,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C14" sqref="C14:C19"/>
     </sheetView>
   </sheetViews>
@@ -584,19 +584,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -632,10 +632,10 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="12">
         <v>0.14923410945010901</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="12">
         <v>0.14923410945010901</v>
       </c>
       <c r="E3" s="4"/>
@@ -645,10 +645,10 @@
       <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="13">
         <v>3.9483129935391197E-3</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="13">
         <v>3.9483129935391197E-3</v>
       </c>
     </row>
@@ -659,8 +659,8 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
         <v>8</v>
@@ -668,8 +668,8 @@
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -678,8 +678,8 @@
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
         <v>12</v>
@@ -687,8 +687,8 @@
       <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -697,8 +697,8 @@
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
         <v>8</v>
@@ -706,8 +706,8 @@
       <c r="G6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -716,8 +716,8 @@
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5" t="s">
         <v>16</v>
@@ -725,8 +725,8 @@
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -735,8 +735,8 @@
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="4"/>
       <c r="F8" s="5" t="s">
         <v>8</v>
@@ -744,8 +744,8 @@
       <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
@@ -760,12 +760,12 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
@@ -790,8 +790,10 @@
       <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="19" t="s">
+      <c r="C14" s="12">
+        <v>0.25909772704723</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="4"/>
@@ -804,8 +806,8 @@
       <c r="B15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
@@ -814,8 +816,8 @@
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
@@ -826,8 +828,8 @@
       <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
@@ -838,8 +840,8 @@
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
@@ -848,8 +850,8 @@
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
@@ -880,7 +882,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C14" sqref="C14:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -896,19 +898,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -944,10 +946,10 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="12">
         <v>0.44</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="12">
         <v>0.44</v>
       </c>
       <c r="E3" s="4"/>
@@ -957,10 +959,10 @@
       <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="12">
         <v>0.26262626262626199</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="12">
         <v>0.26262626262626199</v>
       </c>
     </row>
@@ -971,8 +973,8 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
         <v>8</v>
@@ -980,8 +982,8 @@
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -990,8 +992,8 @@
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
         <v>21</v>
@@ -999,8 +1001,8 @@
       <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -1009,8 +1011,8 @@
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
         <v>8</v>
@@ -1018,8 +1020,8 @@
       <c r="G6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -1028,8 +1030,8 @@
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5" t="s">
         <v>23</v>
@@ -1037,8 +1039,8 @@
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -1047,8 +1049,8 @@
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="4"/>
       <c r="F8" s="5" t="s">
         <v>8</v>
@@ -1056,8 +1058,8 @@
       <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
@@ -1072,12 +1074,12 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
@@ -1102,10 +1104,10 @@
       <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="12">
+        <v>0.49494949494949497</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="4"/>
@@ -1118,8 +1120,8 @@
       <c r="B15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="13"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
@@ -1128,8 +1130,8 @@
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
@@ -1140,8 +1142,8 @@
       <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="13"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
@@ -1152,8 +1154,8 @@
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
@@ -1162,8 +1164,8 @@
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="13"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
@@ -1175,15 +1177,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="H3:H8"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="D3:D8"/>
     <mergeCell ref="I3:I8"/>
     <mergeCell ref="A12:D12"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="H3:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1193,7 +1195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C14" sqref="C14:C19"/>
     </sheetView>
   </sheetViews>
@@ -1211,19 +1213,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1258,10 +1260,10 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="12">
         <v>3.7037037037037E-2</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="12">
         <v>3.7037037037037E-2</v>
       </c>
       <c r="E3" s="4"/>
@@ -1271,10 +1273,10 @@
       <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="12">
         <v>0.25</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="12">
         <v>0.25</v>
       </c>
     </row>
@@ -1285,8 +1287,8 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
         <v>8</v>
@@ -1294,8 +1296,8 @@
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1304,8 +1306,8 @@
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
         <v>28</v>
@@ -1313,8 +1315,8 @@
       <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -1323,8 +1325,8 @@
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
         <v>8</v>
@@ -1332,8 +1334,8 @@
       <c r="G6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -1342,8 +1344,8 @@
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5" t="s">
         <v>31</v>
@@ -1351,8 +1353,8 @@
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -1361,8 +1363,8 @@
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="4"/>
       <c r="F8" s="5" t="s">
         <v>8</v>
@@ -1370,8 +1372,8 @@
       <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
@@ -1386,12 +1388,12 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
@@ -1416,8 +1418,10 @@
       <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="12">
+        <v>0.51851851851851805</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="4"/>
@@ -1430,8 +1434,8 @@
       <c r="B15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="13"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
@@ -1440,8 +1444,8 @@
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
@@ -1452,8 +1456,8 @@
       <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="13"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
@@ -1464,8 +1468,8 @@
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
@@ -1474,8 +1478,8 @@
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="13"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
@@ -1487,15 +1491,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="H3:H8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="I3:I8"/>
     <mergeCell ref="D3:D8"/>
     <mergeCell ref="A12:D12"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="H3:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1506,7 +1510,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1521,17 +1525,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1559,78 +1563,78 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="4"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="4"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="4"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="4"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>

</xml_diff>